<commit_message>
city state country identifier added
</commit_message>
<xml_diff>
--- a/readme.xlsx
+++ b/readme.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
   <si>
     <t>Functional Section</t>
   </si>
@@ -1661,16 +1661,10 @@
     <t>Если часто пользоваться выпадающими списками в меню, то скроллер мышки перестает работать</t>
   </si>
   <si>
-    <t>Я не могу отрисовать карту на страны на новом табе в сетингах - страны, региона и города</t>
-  </si>
-  <si>
     <t>Подумать про логин в сетинги</t>
   </si>
   <si>
     <t>Добавить графики на странице овервью</t>
-  </si>
-  <si>
-    <t>Не могу придумать как загружать карты стран для страницы Региона</t>
   </si>
 </sst>
 </file>
@@ -2310,15 +2304,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2331,9 +2361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2342,39 +2369,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2692,7 +2686,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="60" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -2702,8 +2696,8 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="49" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="61" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2712,16 +2706,16 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="51" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="63" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2730,16 +2724,16 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
-      <c r="C8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -2748,15 +2742,15 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47"/>
-      <c r="C10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="14" t="s">
         <v>18</v>
       </c>
@@ -2766,7 +2760,7 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="48"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="12" t="s">
         <v>19</v>
       </c>
@@ -2774,7 +2768,7 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
@@ -2782,7 +2776,7 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -2794,8 +2788,8 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
-      <c r="C15" s="54" t="s">
+      <c r="B15" s="53"/>
+      <c r="C15" s="65" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2804,16 +2798,16 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-      <c r="C17" s="54" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="65" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -2822,30 +2816,30 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="48"/>
-      <c r="C18" s="56"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
-      <c r="C19" s="56"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="48"/>
-      <c r="C20" s="56"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -2854,7 +2848,7 @@
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="47"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="21" t="s">
         <v>31</v>
       </c>
@@ -2863,8 +2857,8 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="57" t="s">
+      <c r="B23" s="53"/>
+      <c r="C23" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -2872,49 +2866,49 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="47"/>
-      <c r="C24" s="58"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
-      <c r="C25" s="58"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="47"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="22" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="48"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="25" t="s">
@@ -2923,7 +2917,7 @@
       <c r="D30" s="9"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="61"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="20" t="s">
         <v>40</v>
       </c>
@@ -2932,21 +2926,21 @@
       </c>
     </row>
     <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="61"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="25" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="49" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2957,15 +2951,15 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="66"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="30" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="66"/>
-      <c r="C36" s="62" t="s">
+      <c r="B36" s="50"/>
+      <c r="C36" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2973,22 +2967,22 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="66"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="66"/>
-      <c r="C38" s="64"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="48"/>
       <c r="D38" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="66"/>
-      <c r="C39" s="62" t="s">
+      <c r="B39" s="50"/>
+      <c r="C39" s="46" t="s">
         <v>46</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -2996,22 +2990,22 @@
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="66"/>
-      <c r="C40" s="63"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="66"/>
-      <c r="C41" s="64"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="66"/>
-      <c r="C42" s="62" t="s">
+      <c r="B42" s="50"/>
+      <c r="C42" s="46" t="s">
         <v>54</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -3019,22 +3013,22 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="66"/>
-      <c r="C43" s="63"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="47"/>
       <c r="D43" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="66"/>
-      <c r="C44" s="64"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="48"/>
       <c r="D44" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="66"/>
-      <c r="C45" s="62" t="s">
+      <c r="B45" s="50"/>
+      <c r="C45" s="46" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -3042,22 +3036,22 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="66"/>
-      <c r="C46" s="63"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="47"/>
       <c r="D46" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="66"/>
-      <c r="C47" s="64"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="48"/>
       <c r="D47" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="66"/>
-      <c r="C48" s="62" t="s">
+      <c r="B48" s="50"/>
+      <c r="C48" s="46" t="s">
         <v>62</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -3065,22 +3059,22 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="66"/>
-      <c r="C49" s="63"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="47"/>
       <c r="D49" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="66"/>
-      <c r="C50" s="64"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="48"/>
       <c r="D50" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="66"/>
-      <c r="C51" s="62" t="s">
+      <c r="B51" s="50"/>
+      <c r="C51" s="46" t="s">
         <v>66</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -3088,31 +3082,21 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="66"/>
-      <c r="C52" s="63"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="47"/>
       <c r="D52" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="67"/>
-      <c r="C53" s="64"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="48"/>
       <c r="D53" s="7" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B34:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C41"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
@@ -3120,6 +3104,16 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B34:B53"/>
+    <mergeCell ref="C51:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3616,7 +3610,7 @@
   <dimension ref="B3:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,16 +3639,13 @@
       <c r="B5" s="31">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -3662,15 +3653,12 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="31">
         <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few small fixes 4 region settings
</commit_message>
<xml_diff>
--- a/readme.xlsx
+++ b/readme.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="135">
   <si>
     <t>Functional Section</t>
   </si>
@@ -1680,6 +1680,12 @@
   </si>
   <si>
     <t>Пользователь не может менять CountryID, так как оно завязано на картах и без корректного ИД карта просто не появится</t>
+  </si>
+  <si>
+    <t>Пользователь не видит Регионы со статусом "N" в сетингах, такие регионы могут быть обработаны только вручную</t>
+  </si>
+  <si>
+    <t>Пользователь не может менять RegionID, так как оно завязано на картах и без корректного ИД регион не будет подсвечен</t>
   </si>
 </sst>
 </file>
@@ -2319,6 +2325,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2337,54 +2394,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2393,9 +2402,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2704,7 +2710,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="47" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -2714,8 +2720,8 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="53"/>
-      <c r="C5" s="61" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="50" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2724,16 +2730,16 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="53"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2742,16 +2748,16 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="53"/>
-      <c r="C8" s="64"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="53"/>
-      <c r="C9" s="63" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -2760,15 +2766,15 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="53"/>
-      <c r="C10" s="64"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="53"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="14" t="s">
         <v>18</v>
       </c>
@@ -2778,7 +2784,7 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="54"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="12" t="s">
         <v>19</v>
       </c>
@@ -2786,7 +2792,7 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="54"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
@@ -2794,7 +2800,7 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -2806,8 +2812,8 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="65" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="55" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2816,16 +2822,16 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="53"/>
-      <c r="C16" s="66"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="53"/>
-      <c r="C17" s="65" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="55" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -2834,30 +2840,30 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="67"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
-      <c r="C20" s="67"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -2866,7 +2872,7 @@
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="53"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="21" t="s">
         <v>31</v>
       </c>
@@ -2875,8 +2881,8 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="55" t="s">
+      <c r="B23" s="48"/>
+      <c r="C23" s="58" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -2884,49 +2890,49 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="56"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="53"/>
-      <c r="C25" s="56"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="53"/>
-      <c r="C26" s="57"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="53"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="22" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="54"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="54"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="61" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="25" t="s">
@@ -2935,7 +2941,7 @@
       <c r="D30" s="9"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="59"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="20" t="s">
         <v>40</v>
       </c>
@@ -2944,21 +2950,21 @@
       </c>
     </row>
     <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="59"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="59"/>
+      <c r="B33" s="62"/>
       <c r="C33" s="25" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="66" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2969,15 +2975,15 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="50"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="30" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="50"/>
-      <c r="C36" s="46" t="s">
+      <c r="B36" s="67"/>
+      <c r="C36" s="63" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2985,22 +2991,22 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="50"/>
-      <c r="C37" s="47"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="50"/>
-      <c r="C38" s="48"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="65"/>
       <c r="D38" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
-      <c r="C39" s="46" t="s">
+      <c r="B39" s="67"/>
+      <c r="C39" s="63" t="s">
         <v>46</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -3008,22 +3014,22 @@
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="50"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="64"/>
       <c r="D40" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="50"/>
-      <c r="C41" s="48"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="50"/>
-      <c r="C42" s="46" t="s">
+      <c r="B42" s="67"/>
+      <c r="C42" s="63" t="s">
         <v>54</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -3031,22 +3037,22 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="50"/>
-      <c r="C43" s="47"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="64"/>
       <c r="D43" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="50"/>
-      <c r="C44" s="48"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="50"/>
-      <c r="C45" s="46" t="s">
+      <c r="B45" s="67"/>
+      <c r="C45" s="63" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -3054,22 +3060,22 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="50"/>
-      <c r="C46" s="47"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="50"/>
-      <c r="C47" s="48"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="50"/>
-      <c r="C48" s="46" t="s">
+      <c r="B48" s="67"/>
+      <c r="C48" s="63" t="s">
         <v>62</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -3077,22 +3083,22 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="50"/>
-      <c r="C49" s="47"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="64"/>
       <c r="D49" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="50"/>
-      <c r="C50" s="48"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="65"/>
       <c r="D50" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="50"/>
-      <c r="C51" s="46" t="s">
+      <c r="B51" s="67"/>
+      <c r="C51" s="63" t="s">
         <v>66</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -3100,21 +3106,31 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="50"/>
-      <c r="C52" s="47"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="64"/>
       <c r="D52" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="51"/>
-      <c r="C53" s="48"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="65"/>
       <c r="D53" s="7" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B34:B53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
@@ -3122,16 +3138,6 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B34:B53"/>
-    <mergeCell ref="C51:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3282,13 +3288,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="35">
@@ -3384,13 +3390,13 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="71"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
@@ -3483,13 +3489,13 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="71"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
@@ -3537,13 +3543,13 @@
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="71"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
@@ -3625,10 +3631,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C13"/>
+  <dimension ref="B3:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,7 +3700,7 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="46" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3704,6 +3710,22 @@
       </c>
       <c r="C13" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="31">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="31">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>